<commit_message>
fix(): bug image for book dont want to be loadead
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_DePinaRyan.xlsx
+++ b/docs/Journal-de-Travail_DePinaRyan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduvaud-my.sharepoint.com/personal/pa70iyc_eduvaud_ch/Documents/Personal_ETML/P_App/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChinO\Documents\GitHub\Passion_Lecture_App\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="13_ncr:1_{3D35E059-9F52-6940-88C6-EA536396115E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18908B74-71F7-4B47-BE0C-AAEA89A2C687}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E69AABF-CDBE-43BC-8E48-7A22A5F50483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-7170" windowWidth="38640" windowHeight="21120" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t xml:space="preserve">J ai refais mon jdt car l ancien avait beaucoup de soucis, avec les scripts </t>
+  </si>
+  <si>
+    <t>J'ai fait les tags et la partie lecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il reste des bugs comme: on peut pas aller au precedent chapitre </t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1311,7 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1530</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2235,16 +2241,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.3613445378151259E-2</c:v>
+                  <c:v>2.9197080291970802E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8571428571428571</c:v>
+                  <c:v>0.87591240875912413</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1092436974789916</c:v>
+                  <c:v>9.4890510948905105E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4433,7 +4439,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4488,7 +4494,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>29 heures 45 minutes</v>
+        <v>34 heures 15 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4503,15 +4509,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>1500</v>
+        <v>1740</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>285</v>
+        <v>315</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>1785</v>
+        <v>2055</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5021,16 +5027,28 @@
       <c r="G24" s="39"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="63" t="str">
+      <c r="A25" s="63">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="40"/>
+        <v>22</v>
+      </c>
+      <c r="B25" s="34">
+        <v>45806</v>
+      </c>
+      <c r="C25" s="35">
+        <v>4</v>
+      </c>
+      <c r="D25" s="36">
+        <v>30</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="40" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="62" t="str">
@@ -11304,7 +11322,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>3.3613445378151259E-2</v>
+        <v>2.9197080291970802E-2</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11321,15 +11339,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>1320</v>
+        <v>1560</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>1530</v>
+        <v>1800</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11337,11 +11355,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>25 h 30 min</v>
+        <v>30 h 00 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.8571428571428571</v>
+        <v>0.87591240875912413</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11415,7 +11433,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.1092436974789916</v>
+        <v>9.4890510948905105E-2</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11467,26 +11485,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>1500</v>
+        <v>1740</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>285</v>
+        <v>315</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>1785</v>
+        <v>2055</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>31</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>29 h 45 min</v>
+        <v>34 h 15 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.33806818181818182</v>
+        <v>0.38920454545454547</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>31</v>
@@ -11530,6 +11548,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11538,15 +11565,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11751,20 +11769,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>